<commit_message>
moved files into images folder and code into code file
</commit_message>
<xml_diff>
--- a/Project/Gantt project planner.xlsx
+++ b/Project/Gantt project planner.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="26">
   <si>
     <t>ACTIVITY</t>
   </si>
@@ -183,6 +183,9 @@
   </si>
   <si>
     <t>Create Checkout page</t>
+  </si>
+  <si>
+    <t>Create Cart Class</t>
   </si>
 </sst>
 </file>
@@ -1003,7 +1006,7 @@
   <dimension ref="B1:BO30"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -1494,12 +1497,24 @@
       </c>
     </row>
     <row r="14" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B14" s="6"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="8"/>
+      <c r="B14" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="7">
+        <v>1</v>
+      </c>
+      <c r="D14" s="7">
+        <v>3</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G14" s="8">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B15" s="6"/>

</xml_diff>